<commit_message>
added ltu and lnu data, some parts reamin to be done
</commit_message>
<xml_diff>
--- a/data/ltu/original_data/ltu_2021.xlsx
+++ b/data/ltu/original_data/ltu_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilla/Documents/repos/openapc-se/data/ltu/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BCA330-77FF-3647-B429-520019341C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166341FB-7E62-2848-96D7-4C20DD74EAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="6260" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1085,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>